<commit_message>
Created a Class based system
</commit_message>
<xml_diff>
--- a/results/111.xlsx
+++ b/results/111.xlsx
@@ -480,7 +480,7 @@
         <v>7.5</v>
       </c>
       <c r="C2">
-        <v>5.846012804034368</v>
+        <v>7.078978318681481</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -491,7 +491,7 @@
         <v>22.5</v>
       </c>
       <c r="C3">
-        <v>5.846012804034368</v>
+        <v>7.078978318681481</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -502,7 +502,7 @@
         <v>37.5</v>
       </c>
       <c r="C4">
-        <v>5.846012804034368</v>
+        <v>7.078978318681481</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -513,7 +513,7 @@
         <v>52.5</v>
       </c>
       <c r="C5">
-        <v>5.846012804034368</v>
+        <v>7.078978318681481</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -524,7 +524,7 @@
         <v>67.5</v>
       </c>
       <c r="C6">
-        <v>5.846012804034368</v>
+        <v>7.078978318681481</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -535,7 +535,7 @@
         <v>82.5</v>
       </c>
       <c r="C7">
-        <v>5.846012804034368</v>
+        <v>7.078978318681481</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -546,7 +546,7 @@
         <v>97.5</v>
       </c>
       <c r="C8">
-        <v>5.846012804034368</v>
+        <v>7.078978318681481</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -557,7 +557,7 @@
         <v>112.5</v>
       </c>
       <c r="C9">
-        <v>5.846012804034368</v>
+        <v>7.078978318681481</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -568,7 +568,7 @@
         <v>127.5</v>
       </c>
       <c r="C10">
-        <v>5.846012804034368</v>
+        <v>7.078978318681481</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -579,7 +579,7 @@
         <v>142.5</v>
       </c>
       <c r="C11">
-        <v>5.846012804034368</v>
+        <v>7.078978318681481</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -590,7 +590,7 @@
         <v>157.5</v>
       </c>
       <c r="C12">
-        <v>5.846012804034368</v>
+        <v>7.078978318681481</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -601,7 +601,7 @@
         <v>172.5</v>
       </c>
       <c r="C13">
-        <v>5.846012804034368</v>
+        <v>7.078978318681481</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -612,7 +612,7 @@
         <v>187.5</v>
       </c>
       <c r="C14">
-        <v>5.846012804034368</v>
+        <v>7.434441912803813</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -623,7 +623,7 @@
         <v>202.5</v>
       </c>
       <c r="C15">
-        <v>5.846012804034368</v>
+        <v>7.301143065007938</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -634,7 +634,7 @@
         <v>217.5</v>
       </c>
       <c r="C16">
-        <v>5.846012804034368</v>
+        <v>7.301143065007938</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -645,7 +645,7 @@
         <v>232.5</v>
       </c>
       <c r="C17">
-        <v>5.846012804034368</v>
+        <v>7.145627742579418</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -656,7 +656,7 @@
         <v>247.5</v>
       </c>
       <c r="C18">
-        <v>5.846012804034368</v>
+        <v>7.545524285967042</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -667,7 +667,7 @@
         <v>262.5</v>
       </c>
       <c r="C19">
-        <v>5.846012804034368</v>
+        <v>7.412225438171168</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -678,7 +678,7 @@
         <v>277.5</v>
       </c>
       <c r="C20">
-        <v>5.846012804034368</v>
+        <v>7.234493641110001</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -689,7 +689,7 @@
         <v>292.5</v>
       </c>
       <c r="C21">
-        <v>5.846012804034368</v>
+        <v>7.434441912803813</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -700,7 +700,7 @@
         <v>307.5</v>
       </c>
       <c r="C22">
-        <v>5.846012804034368</v>
+        <v>7.723256083028208</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -711,7 +711,7 @@
         <v>322.5</v>
       </c>
       <c r="C23">
-        <v>5.846012804034368</v>
+        <v>7.434441912803813</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -722,7 +722,7 @@
         <v>337.5</v>
       </c>
       <c r="C24">
-        <v>5.846012804034368</v>
+        <v>7.234493641110001</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -733,7 +733,7 @@
         <v>352.5</v>
       </c>
       <c r="C25">
-        <v>5.846012804034368</v>
+        <v>7.523307811334396</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -744,7 +744,7 @@
         <v>367.5</v>
       </c>
       <c r="C26">
-        <v>5.846012804034368</v>
+        <v>7.278926590375294</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -755,7 +755,7 @@
         <v>382.5</v>
       </c>
       <c r="C27">
-        <v>5.846012804034368</v>
+        <v>7.234493641110001</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -766,7 +766,7 @@
         <v>397.5</v>
       </c>
       <c r="C28">
-        <v>5.846012804034368</v>
+        <v>7.234493641110001</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -777,7 +777,7 @@
         <v>412.5</v>
       </c>
       <c r="C29">
-        <v>5.846012804034368</v>
+        <v>7.234493641110001</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -788,7 +788,7 @@
         <v>427.5</v>
       </c>
       <c r="C30">
-        <v>5.846012804034368</v>
+        <v>7.7676890322935</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -799,7 +799,7 @@
         <v>442.5</v>
       </c>
       <c r="C31">
-        <v>7.614281372149604</v>
+        <v>7.367792488905875</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -810,7 +810,7 @@
         <v>457.5</v>
       </c>
       <c r="C32">
-        <v>8.892547806931702</v>
+        <v>8.634131542966683</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -821,7 +821,7 @@
         <v>472.5</v>
       </c>
       <c r="C33">
-        <v>10.08559647939499</v>
+        <v>10.65583073453745</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -832,7 +832,7 @@
         <v>487.5</v>
       </c>
       <c r="C34">
-        <v>10.44777196924992</v>
+        <v>13.03299352023054</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -843,7 +843,7 @@
         <v>502.5</v>
       </c>
       <c r="C35">
-        <v>11.32125403301769</v>
+        <v>14.01051840406696</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -854,7 +854,7 @@
         <v>517.5</v>
       </c>
       <c r="C36">
-        <v>12.06690945330724</v>
+        <v>13.98830192943431</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -865,7 +865,7 @@
         <v>532.5</v>
       </c>
       <c r="C37">
-        <v>13.13213148229233</v>
+        <v>13.89943603090373</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -876,7 +876,7 @@
         <v>547.5</v>
       </c>
       <c r="C38">
-        <v>13.72865581852397</v>
+        <v>13.56618891141404</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -887,7 +887,7 @@
         <v>562.5</v>
       </c>
       <c r="C39">
-        <v>14.0695268677992</v>
+        <v>14.29933257429135</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -898,7 +898,7 @@
         <v>577.5</v>
       </c>
       <c r="C40">
-        <v>13.94170022432099</v>
+        <v>13.96608545480166</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -909,7 +909,7 @@
         <v>592.5</v>
       </c>
       <c r="C41">
-        <v>13.72865581852397</v>
+        <v>12.01103568712884</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -920,7 +920,7 @@
         <v>607.5</v>
       </c>
       <c r="C42">
-        <v>12.98300039823441</v>
+        <v>9.633872901435744</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -931,7 +931,7 @@
         <v>622.5</v>
       </c>
       <c r="C43">
-        <v>12.7486515518577</v>
+        <v>8.07871967715054</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -942,7 +942,7 @@
         <v>637.5</v>
       </c>
       <c r="C44">
-        <v>11.23603627069888</v>
+        <v>7.434441912803813</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -953,7 +953,7 @@
         <v>652.5</v>
       </c>
       <c r="C45">
-        <v>9.829943192438574</v>
+        <v>7.523307811334396</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -964,7 +964,7 @@
         <v>667.5</v>
       </c>
       <c r="C46">
-        <v>8.849938925772298</v>
+        <v>7.234493641110001</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -975,7 +975,7 @@
         <v>682.5</v>
       </c>
       <c r="C47">
-        <v>6.847321511280345</v>
+        <v>7.234493641110001</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -986,7 +986,7 @@
         <v>697.5</v>
       </c>
       <c r="C48">
-        <v>5.846012804034368</v>
+        <v>7.278926590375294</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -997,7 +997,7 @@
         <v>712.5</v>
       </c>
       <c r="C49">
-        <v>5.846012804034368</v>
+        <v>7.523307811334396</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -1008,7 +1008,7 @@
         <v>727.5</v>
       </c>
       <c r="C50">
-        <v>5.846012804034368</v>
+        <v>7.523307811334396</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -1019,7 +1019,7 @@
         <v>742.5</v>
       </c>
       <c r="C51">
-        <v>5.846012804034368</v>
+        <v>7.234493641110001</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -1030,7 +1030,7 @@
         <v>757.5</v>
       </c>
       <c r="C52">
-        <v>5.846012804034368</v>
+        <v>7.19006069184471</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -1041,7 +1041,7 @@
         <v>772.5</v>
       </c>
       <c r="C53">
-        <v>5.846012804034368</v>
+        <v>7.234493641110001</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -1052,7 +1052,7 @@
         <v>787.5</v>
       </c>
       <c r="C54">
-        <v>5.846012804034368</v>
+        <v>7.145627742579418</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -1063,7 +1063,7 @@
         <v>802.5</v>
       </c>
       <c r="C55">
-        <v>5.846012804034368</v>
+        <v>7.145627742579418</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -1074,7 +1074,7 @@
         <v>817.5</v>
       </c>
       <c r="C56">
-        <v>5.846012804034368</v>
+        <v>7.078978318681481</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1085,7 +1085,7 @@
         <v>832.5</v>
       </c>
       <c r="C57">
-        <v>5.846012804034368</v>
+        <v>7.078978318681481</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -1096,7 +1096,7 @@
         <v>847.5</v>
       </c>
       <c r="C58">
-        <v>5.846012804034368</v>
+        <v>7.078978318681481</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -1107,7 +1107,7 @@
         <v>862.5</v>
       </c>
       <c r="C59">
-        <v>5.846012804034368</v>
+        <v>7.078978318681481</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -1118,7 +1118,7 @@
         <v>877.5</v>
       </c>
       <c r="C60">
-        <v>5.846012804034368</v>
+        <v>7.078978318681481</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -1129,7 +1129,7 @@
         <v>892.5</v>
       </c>
       <c r="C61">
-        <v>5.846012804034368</v>
+        <v>7.078978318681481</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -1140,7 +1140,7 @@
         <v>907.5</v>
       </c>
       <c r="C62">
-        <v>5.846012804034368</v>
+        <v>7.078978318681481</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -1151,7 +1151,7 @@
         <v>922.5</v>
       </c>
       <c r="C63">
-        <v>5.846012804034368</v>
+        <v>7.078978318681481</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -1162,7 +1162,7 @@
         <v>937.5</v>
       </c>
       <c r="C64">
-        <v>5.846012804034368</v>
+        <v>7.078978318681481</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -1173,7 +1173,7 @@
         <v>952.5</v>
       </c>
       <c r="C65">
-        <v>5.846012804034368</v>
+        <v>7.078978318681481</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -1184,7 +1184,7 @@
         <v>967.5</v>
       </c>
       <c r="C66">
-        <v>5.846012804034368</v>
+        <v>7.078978318681481</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -1195,7 +1195,7 @@
         <v>982.5</v>
       </c>
       <c r="C67">
-        <v>5.846012804034368</v>
+        <v>7.078978318681481</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -1206,7 +1206,7 @@
         <v>997.5</v>
       </c>
       <c r="C68">
-        <v>5.846012804034368</v>
+        <v>7.078978318681481</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -1217,7 +1217,7 @@
         <v>1012.5</v>
       </c>
       <c r="C69">
-        <v>5.846012804034368</v>
+        <v>7.078978318681481</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -1228,7 +1228,7 @@
         <v>1027.5</v>
       </c>
       <c r="C70">
-        <v>5.846012804034368</v>
+        <v>7.078978318681481</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -1239,7 +1239,7 @@
         <v>1042.5</v>
       </c>
       <c r="C71">
-        <v>5.846012804034368</v>
+        <v>7.078978318681481</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -1250,7 +1250,7 @@
         <v>1057.5</v>
       </c>
       <c r="C72">
-        <v>5.846012804034368</v>
+        <v>7.078978318681481</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -1261,7 +1261,7 @@
         <v>1072.5</v>
       </c>
       <c r="C73">
-        <v>5.846012804034368</v>
+        <v>7.078978318681481</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -1272,7 +1272,7 @@
         <v>1087.5</v>
       </c>
       <c r="C74">
-        <v>5.846012804034368</v>
+        <v>7.078978318681481</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -1283,7 +1283,7 @@
         <v>1102.5</v>
       </c>
       <c r="C75">
-        <v>5.846012804034368</v>
+        <v>7.078978318681481</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -1294,7 +1294,7 @@
         <v>1117.5</v>
       </c>
       <c r="C76">
-        <v>5.846012804034368</v>
+        <v>7.078978318681481</v>
       </c>
     </row>
   </sheetData>

</xml_diff>